<commit_message>
Update zoning code match comparison.xlsx
</commit_message>
<xml_diff>
--- a/doc-reader/data/zoning code match count/zoning code match comparison.xlsx
+++ b/doc-reader/data/zoning code match count/zoning code match comparison.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinyi/Documents/GitHub/freddie-mac/doc-reader/data/zoning code match count/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA08E3D-C990-3C48-8B3F-8418722E741A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B3D4A3-950B-C54B-B5F5-DD0A545C8D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="3460" windowWidth="27440" windowHeight="16440" xr2:uid="{544BC5F3-E72D-1749-94A7-38DCEE0B7A9D}"/>
+    <workbookView xWindow="1420" yWindow="840" windowWidth="31020" windowHeight="19720" xr2:uid="{544BC5F3-E72D-1749-94A7-38DCEE0B7A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="3" r:id="rId1"/>
     <sheet name="Joey" sheetId="1" r:id="rId2"/>
     <sheet name="Xinyi" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparison!$A$1:$Q$62</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="410">
   <si>
     <t>idx</t>
   </si>
@@ -948,430 +951,432 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ER-1, ER-2, ER-3, SR-2, SR-3, SR-4, SR-5, SR-6, MH-1, OR, B-1, B-2, B-3, B-4, I-1, I-2, P-1, W-B, PD, DT-O</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HINSDALE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/hinsdaleil/latest/hinsdale_il_zoning/0-0-0-39</t>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, R-4, R-5, R-6, B-1, B-2, B-3, O-1, O-2, O-3, HS, OS, IB, DR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MINOOKA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/minookail/latest/minooka_il/0-0-0-5147</t>
+  </si>
+  <si>
+    <t>A, R1, R1A, R2, R3, R4, R4A, R5, R6, B1, B2, M1, M2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LINDENHURST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E, SE, S, R-1, R-2, R-3, R-4, NB, CB, CBR-2, PBC, O, BK, M, I, RO, Planned Unit Development Districts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MANHATTAN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-1, CR, ER, GR, R-1, R-2, R-3, R-4, R-5, R-6, C-1, C-2, C-3, CBD, BP, DD, I-1, I-2, I-3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WINNETKA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/winnetka/latest/winnetka_il/0-0-0-26184#JD_Chapter17.08</t>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/manhattanil/latest/manhattan_il/0-0-0-2889</t>
+  </si>
+  <si>
+    <t>R-5, R-4, R-3, R-2, R-1, B-1, B-2, C-1, C-2, D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAKE ZURICH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/lakezurichil/latest/lakezurich_il/0-0-0-14105</t>
+  </si>
+  <si>
+    <t>R-1/2, R-3, R-4, R-5, R-6, B-1, B-2, B-3, O-1, O-2, O-3, I, OS, IB, LP, DR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WINTHROP HARBOR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/winthropharbor/latest/winthropharbor_il/0-0-0-40225</t>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, R-4, R-5, B-1, B1-M, B-2, B-3, B-4, B-5, I-1, I-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHATHAM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/chatham/latest/chatham_il/0-0-0-6880</t>
+  </si>
+  <si>
+    <t>R-1, R1A, R-2, R-3, R-3A, RM-4, RO-5, B-1, B-2, I-1, I-2, PUD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOKENA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/mokenail/latest/mokena_il/0-0-0-6536</t>
+  </si>
+  <si>
+    <t>E-1, R-1, R-2, R-3, R-4, R-5, R-6, C-1, C-1A, C-2, C-3, C-4, O-1, O-2, I-1, I-2, I-3, A-1, P-1, OR-1, TOD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WINFIELD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ER-1, ER-2, ER-3, R-1, R-1A, R-1B, R-2, R-3, R-4A, R-4B, R-5, R-6, R-7, SC-PD, TC, B-1, B-2, B-2A, RW-PD, P-1, L-1, PUD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JERSEYVILLE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/jerseyvilleil/latest/jerseyville_il/0-0-0-3842#JD_11-4-1</t>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, R-4, R-5, R-6, R-7, B-1, B-2, B-3, M-1, M-2, M-3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCKPORT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/lockport/latest/lockport_il/0-0-0-83483</t>
+  </si>
+  <si>
+    <t>A-1, E-R, R-O, R-1, R-2, R-3, R-4, C-1, C-2, C-2T, C-3, C-4, O-1, O-2, M-1, M-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROMEOVILLE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/romeoville/latest/romeoville_il/0-0-0-17963</t>
+  </si>
+  <si>
+    <t>A-1, E-R, R-1, R-2, R-3, R-4, R-5, R-5A, R-6, R-7, B-1, B-2, B-3, B-4, P-1, P-B, DD, M-R, M-1, M-2, AD-1, AD-2, U-D, FP-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DYER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/dyer/latest/dyer_in/0-0-0-8285</t>
+  </si>
+  <si>
+    <t>RD, R-1, R-2, R-3, R-4, R-5M, B-1, B-2, B-3, I, R/B, PUD, SUD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAST GRAND RAPIDS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, MFR, C-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/eastgrandrapidsmi/latest/eastgrandrapids_mi/0-0-0-3146</t>
+  </si>
+  <si>
+    <t>GARDEN CITY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, O-1, C-1, C-2, C-3, CBD, M-1, PD, VP, PR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FARMINGTON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/farmingtonmn/latest/farmington_mn/0-0-0-5596#JD_10-5-2</t>
+  </si>
+  <si>
+    <t>A-1, R-1, R-2, R-3, R-4, R-D, B-1, B-2, B-3, SSMU, MUCI, MUCR, I, P/OS, PUD, DC-O, HW3-O, SS-O</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BROOK PARK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/brookpark/latest/brookpark_oh/0-0-0-40686</t>
+  </si>
+  <si>
+    <t>NOTE: Different districts for use, height, and area</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HIGHLAND HEIGHTS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/highlandhts/latest/highlandhts_oh/0-0-0-17621#1121</t>
+  </si>
+  <si>
+    <t>U-1, U-2, U-3, P, O-B, L-B, M-S, G-B, P-C-M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPRINGFIELD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/springfield/latest/springfield_oh/0-0-0-11623</t>
+  </si>
+  <si>
+    <t>A, RR-1, RS-5, RS-8, RFBH, RM-12, RM-20, CN-2, RM-44, RM-44A, CO-1, CN-1, CC-2, EC-1, CB-10, CH-1, CI-1, RDP, M-1, M-2, G, OFP, OHP, OPD, CC-2A, UCOD, UCED, DMC, PD, EECPOD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MENTOR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/mentor/latest/mentor_oh/0-0-0-18059</t>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, R-4, R-5, R-10, RMH, C-1, C-2, OV, B-1, B-2, B-3, PUD, M-1, M-2, MRD, MIP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WICKLIFFE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/wickliffe/latest/wickliffe_oh/0-0-0-23303</t>
+  </si>
+  <si>
+    <t>OS, INS, R1-100, R1-75, R1-60, R1-50, R2F, RMF, S/A, OB, GB, TC, CM, I</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMHERST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/amherst/latest/amherst_oh/0-0-0-13431#JD_PartEleven-PlanningandZoningCode-TitleFive</t>
+  </si>
+  <si>
+    <t>R-1, PD, R-2, R-3, C-1, C-2, C-3, I-1, M-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORTH RIDGEVILLE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, R-4, R-5, RS-1, RS-2, B-1, B-2, B-3, B-4, B-5, I-1, I-2, I-3, PCD, SDD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAIRFIELD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/fairfield/latest/fairfield_oh/0-0-0-11495</t>
+  </si>
+  <si>
+    <t>A-1, R-0, R-1, R-2, R-3, R-4, B-1, C-4, C-1, C-2, C-2A, C-2B, C-3, C-3A, M-1, M-1A, M-2, M-2A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>color</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOUTH EUCLID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/southeuclid/latest/seuclid_oh/0-0-0-10364</t>
+  </si>
+  <si>
+    <t>R-75, R-60, R-50, R-40, M-F, R-O, C-1, C-2, C-3, M-1, M-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MONTGOMERY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/montgomery/latest/montgom_oh/0-0-0-37923#JD_Chapter151.01</t>
+  </si>
+  <si>
+    <t>A, B, C, D-2, D-3, O, OC, L-B, G-B, OM, OMG, H-O</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WYOMING</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/wyoming/latest/wyoming_oh/0-0-0-20416#JD_1145</t>
+  </si>
+  <si>
+    <t>AAAA, AAA, AA, A, B, C-1, C-2, C-3, E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/avonoh/latest/avon_oh/0-0-0-46315</t>
+  </si>
+  <si>
+    <t>R-1, R-2, R-3, C-1, C-2, C-3, C-4, O-1, O-2, M-1, M-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>STRUTHERS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/struthers/latest/struthers_oh/0-0-0-12770</t>
+  </si>
+  <si>
+    <t>Residence A, Residence B, Residence C, Residence C-1, Commercial A, Commercial B, Industrial A, Industrial B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEVEN HILLS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/sevenhills/latest/sevenhills_oh/0-0-0-17227</t>
+  </si>
+  <si>
+    <t>NOTE: ALL TEXTS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MACEDONIA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/macedonia/latest/macedonia_oh/0-0-0-14557</t>
+  </si>
+  <si>
+    <t>R, B-1, B-2, B-3, B-4, I, R-P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JAMES ISLAND</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/jamesisland/latest/jamesisland_sc/0-0-0-3360#JD_153.065</t>
+  </si>
+  <si>
+    <t>NRM-25, AG-5, AGR, RSL, RSM, MHS, OR, OG, CN, CC, I, PD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COLLIERVILLE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/collierville/latest/collierv_tn/0-0-0-42717#JD_151.020</t>
+  </si>
+  <si>
+    <t>R-1, R-1A, R-2, R-2A, R-3, R-3A, R-4, T, R-TH, RL, R-25, R-L1, FAR, NC, MPO, SCC, CB, GC, RI, GI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOUTH WEBER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://codelibrary.amlegal.com/codes/southweberut/latest/southweber_ut/0-0-0-3250</t>
+  </si>
+  <si>
+    <t>R-M, R-LM, R-7, R-L, A, A-10, C, C-H, T-1, N-R, P-O,  L-I, C-R, C-O, B-C, R-P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HERRIMAN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-.25, A-.5, A-1, R-1-10, R-1-15, R-1-21, R-1-43, R-2-10, R-2-15, R-M, FR-1, FR-2.5, FR-5, FR-10, FR-20, RC, C-1, C-2, OP, T-M, M-1, MU, MU-2, EC, H, PD, W, VMU, AMSD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEDAR HILLS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-1-11,000, R-1-15,000, PD-1, H-1, SC-1, RR-1-20,000, PR 2,2, PR 3.4, TR-1, PF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SANTA CLARA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS, RA, R-1-10, R-1-10/RA, Commerical Zone, Planned development residential zone, Planned commercial development zone, Planned office and institutional development zone, Planned industrial development zone, Historic district/mixed use zone, HD, HP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>https://codelibrary.amlegal.com/codes/bartlettil/latest/bartlett_il/0-0-0-9499#JD_10-4-1</t>
-  </si>
-  <si>
-    <t>ER-1, ER-2, ER-3, SR-2, SR-3, SR-4, SR-5, SR-6, MH-1, OR, B-1, B-2, B-3, B-4, I-1, I-2, P-1, W-B, PD, DT-O</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HINSDALE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/hinsdaleil/latest/hinsdale_il_zoning/0-0-0-39</t>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, R-4, R-5, R-6, B-1, B-2, B-3, O-1, O-2, O-3, HS, OS, IB, DR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MINOOKA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/minookail/latest/minooka_il/0-0-0-5147</t>
-  </si>
-  <si>
-    <t>A, R1, R1A, R2, R3, R4, R4A, R5, R6, B1, B2, M1, M2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LINDENHURST</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E, SE, S, R-1, R-2, R-3, R-4, NB, CB, CBR-2, PBC, O, BK, M, I, RO, Planned Unit Development Districts</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MANHATTAN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-1, CR, ER, GR, R-1, R-2, R-3, R-4, R-5, R-6, C-1, C-2, C-3, CBD, BP, DD, I-1, I-2, I-3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WINNETKA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/winnetka/latest/winnetka_il/0-0-0-26184#JD_Chapter17.08</t>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/manhattanil/latest/manhattan_il/0-0-0-2889</t>
-  </si>
-  <si>
-    <t>R-5, R-4, R-3, R-2, R-1, B-1, B-2, C-1, C-2, D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LAKE ZURICH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/lakezurichil/latest/lakezurich_il/0-0-0-14105</t>
-  </si>
-  <si>
-    <t>R-1/2, R-3, R-4, R-5, R-6, B-1, B-2, B-3, O-1, O-2, O-3, I, OS, IB, LP, DR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WINTHROP HARBOR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/winthropharbor/latest/winthropharbor_il/0-0-0-40225</t>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, R-4, R-5, B-1, B1-M, B-2, B-3, B-4, B-5, I-1, I-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHATHAM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/chatham/latest/chatham_il/0-0-0-6880</t>
-  </si>
-  <si>
-    <t>R-1, R1A, R-2, R-3, R-3A, RM-4, RO-5, B-1, B-2, I-1, I-2, PUD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MOKENA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/mokenail/latest/mokena_il/0-0-0-6536</t>
-  </si>
-  <si>
-    <t>E-1, R-1, R-2, R-3, R-4, R-5, R-6, C-1, C-1A, C-2, C-3, C-4, O-1, O-2, I-1, I-2, I-3, A-1, P-1, OR-1, TOD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WINFIELD</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>https://codelibrary.amlegal.com/codes/winfieldil/latest/winfield_il/0-0-0-7209</t>
-  </si>
-  <si>
-    <t>ER-1, ER-2, ER-3, R-1, R-1A, R-1B, R-2, R-3, R-4A, R-4B, R-5, R-6, R-7, SC-PD, TC, B-1, B-2, B-2A, RW-PD, P-1, L-1, PUD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JERSEYVILLE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/jerseyvilleil/latest/jerseyville_il/0-0-0-3842#JD_11-4-1</t>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, R-4, R-5, R-6, R-7, B-1, B-2, B-3, M-1, M-2, M-3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOCKPORT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/lockport/latest/lockport_il/0-0-0-83483</t>
-  </si>
-  <si>
-    <t>A-1, E-R, R-O, R-1, R-2, R-3, R-4, C-1, C-2, C-2T, C-3, C-4, O-1, O-2, M-1, M-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ROMEOVILLE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/romeoville/latest/romeoville_il/0-0-0-17963</t>
-  </si>
-  <si>
-    <t>A-1, E-R, R-1, R-2, R-3, R-4, R-5, R-5A, R-6, R-7, B-1, B-2, B-3, B-4, P-1, P-B, DD, M-R, M-1, M-2, AD-1, AD-2, U-D, FP-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DYER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/dyer/latest/dyer_in/0-0-0-8285</t>
-  </si>
-  <si>
-    <t>RD, R-1, R-2, R-3, R-4, R-5M, B-1, B-2, B-3, I, R/B, PUD, SUD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EAST GRAND RAPIDS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, MFR, C-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/eastgrandrapidsmi/latest/eastgrandrapids_mi/0-0-0-3146</t>
-  </si>
-  <si>
-    <t>GARDEN CITY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, O-1, C-1, C-2, C-3, CBD, M-1, PD, VP, PR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FARMINGTON</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/farmingtonmn/latest/farmington_mn/0-0-0-5596#JD_10-5-2</t>
-  </si>
-  <si>
-    <t>A-1, R-1, R-2, R-3, R-4, R-D, B-1, B-2, B-3, SSMU, MUCI, MUCR, I, P/OS, PUD, DC-O, HW3-O, SS-O</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BROOK PARK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/brookpark/latest/brookpark_oh/0-0-0-40686</t>
-  </si>
-  <si>
-    <t>NOTE: Different districts for use, height, and area</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HIGHLAND HEIGHTS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/highlandhts/latest/highlandhts_oh/0-0-0-17621#1121</t>
-  </si>
-  <si>
-    <t>U-1, U-2, U-3, P, O-B, L-B, M-S, G-B, P-C-M</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPRINGFIELD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/springfield/latest/springfield_oh/0-0-0-11623</t>
-  </si>
-  <si>
-    <t>A, RR-1, RS-5, RS-8, RFBH, RM-12, RM-20, CN-2, RM-44, RM-44A, CO-1, CN-1, CC-2, EC-1, CB-10, CH-1, CI-1, RDP, M-1, M-2, G, OFP, OHP, OPD, CC-2A, UCOD, UCED, DMC, PD, EECPOD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MENTOR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/mentor/latest/mentor_oh/0-0-0-18059</t>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, R-4, R-5, R-10, RMH, C-1, C-2, OV, B-1, B-2, B-3, PUD, M-1, M-2, MRD, MIP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WICKLIFFE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/wickliffe/latest/wickliffe_oh/0-0-0-23303</t>
-  </si>
-  <si>
-    <t>OS, INS, R1-100, R1-75, R1-60, R1-50, R2F, RMF, S/A, OB, GB, TC, CM, I</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMHERST</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/amherst/latest/amherst_oh/0-0-0-13431#JD_PartEleven-PlanningandZoningCode-TitleFive</t>
-  </si>
-  <si>
-    <t>R-1, PD, R-2, R-3, C-1, C-2, C-3, I-1, M-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NORTH RIDGEVILLE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, R-4, R-5, RS-1, RS-2, B-1, B-2, B-3, B-4, B-5, I-1, I-2, I-3, PCD, SDD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAIRFIELD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/fairfield/latest/fairfield_oh/0-0-0-11495</t>
-  </si>
-  <si>
-    <t>A-1, R-0, R-1, R-2, R-3, R-4, B-1, C-4, C-1, C-2, C-2A, C-2B, C-3, C-3A, M-1, M-1A, M-2, M-2A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>color</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orange</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOUTH EUCLID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/southeuclid/latest/seuclid_oh/0-0-0-10364</t>
-  </si>
-  <si>
-    <t>R-75, R-60, R-50, R-40, M-F, R-O, C-1, C-2, C-3, M-1, M-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MONTGOMERY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/montgomery/latest/montgom_oh/0-0-0-37923#JD_Chapter151.01</t>
-  </si>
-  <si>
-    <t>A, B, C, D-2, D-3, O, OC, L-B, G-B, OM, OMG, H-O</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>WYOMING</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/wyoming/latest/wyoming_oh/0-0-0-20416#JD_1145</t>
-  </si>
-  <si>
-    <t>AAAA, AAA, AA, A, B, C-1, C-2, C-3, E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AVON</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/avonoh/latest/avon_oh/0-0-0-46315</t>
-  </si>
-  <si>
-    <t>R-1, R-2, R-3, C-1, C-2, C-3, C-4, O-1, O-2, M-1, M-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>STRUTHERS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/struthers/latest/struthers_oh/0-0-0-12770</t>
-  </si>
-  <si>
-    <t>Residence A, Residence B, Residence C, Residence C-1, Commercial A, Commercial B, Industrial A, Industrial B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEVEN HILLS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/sevenhills/latest/sevenhills_oh/0-0-0-17227</t>
-  </si>
-  <si>
-    <t>NOTE: ALL TEXTS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MACEDONIA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/macedonia/latest/macedonia_oh/0-0-0-14557</t>
-  </si>
-  <si>
-    <t>R, B-1, B-2, B-3, B-4, I, R-P</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>JAMES ISLAND</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/jamesisland/latest/jamesisland_sc/0-0-0-3360#JD_153.065</t>
-  </si>
-  <si>
-    <t>NRM-25, AG-5, AGR, RSL, RSM, MHS, OR, OG, CN, CC, I, PD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>COLLIERVILLE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/collierville/latest/collierv_tn/0-0-0-42717#JD_151.020</t>
-  </si>
-  <si>
-    <t>R-1, R-1A, R-2, R-2A, R-3, R-3A, R-4, T, R-TH, RL, R-25, R-L1, FAR, NC, MPO, SCC, CB, GC, RI, GI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOUTH WEBER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://codelibrary.amlegal.com/codes/southweberut/latest/southweber_ut/0-0-0-3250</t>
-  </si>
-  <si>
-    <t>R-M, R-LM, R-7, R-L, A, A-10, C, C-H, T-1, N-R, P-O,  L-I, C-R, C-O, B-C, R-P</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HERRIMAN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-.25, A-.5, A-1, R-1-10, R-1-15, R-1-21, R-1-43, R-2-10, R-2-15, R-M, FR-1, FR-2.5, FR-5, FR-10, FR-20, RC, C-1, C-2, OP, T-M, M-1, MU, MU-2, EC, H, PD, W, VMU, AMSD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CEDAR HILLS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-1-11,000, R-1-15,000, PD-1, H-1, SC-1, RR-1-20,000, PR 2,2, PR 3.4, TR-1, PF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SANTA CLARA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OS, RA, R-1-10, R-1-10/RA, Commerical Zone, Planned development residential zone, Planned commercial development zone, Planned office and institutional development zone, Planned industrial development zone, Historic district/mixed use zone, HD, HP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1513,10 +1518,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1819,10 +1820,10 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1849,7 +1850,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F1" t="s">
         <v>243</v>
@@ -1899,7 +1900,7 @@
         <v>247</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F2">
         <v>30</v>
@@ -1955,7 +1956,7 @@
         <v>253</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F3">
         <v>13</v>
@@ -2011,7 +2012,7 @@
         <v>285</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F4">
         <v>34</v>
@@ -2173,7 +2174,7 @@
         <v>294</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -2183,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2207,8 +2208,8 @@
       <c r="O7" t="s">
         <v>37</v>
       </c>
-      <c r="P7" t="s">
-        <v>295</v>
+      <c r="P7" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -2222,10 +2223,10 @@
         <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F8">
         <v>32</v>
@@ -2235,7 +2236,7 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I8" s="3">
         <f>14/F8</f>
@@ -2264,7 +2265,7 @@
         <v>40</v>
       </c>
       <c r="P8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2278,10 +2279,10 @@
         <v>41</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2291,7 +2292,7 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -2318,7 +2319,7 @@
         <v>44</v>
       </c>
       <c r="P9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2332,10 +2333,10 @@
         <v>45</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F10">
         <v>24</v>
@@ -2345,7 +2346,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I10" s="3">
         <f>8/F10</f>
@@ -2385,7 +2386,7 @@
         <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F11">
         <v>18</v>
@@ -2395,7 +2396,7 @@
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I11" s="3">
         <f>17/F11</f>
@@ -2424,7 +2425,7 @@
         <v>52</v>
       </c>
       <c r="P11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2438,7 +2439,7 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F12">
         <v>9</v>
@@ -2448,7 +2449,7 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I12" s="3">
         <f>9/F12</f>
@@ -2477,7 +2478,7 @@
         <v>55</v>
       </c>
       <c r="P12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2491,10 +2492,10 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -2504,7 +2505,7 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -2528,8 +2529,8 @@
       <c r="O13" t="s">
         <v>58</v>
       </c>
-      <c r="P13" t="s">
-        <v>324</v>
+      <c r="P13" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2543,10 +2544,10 @@
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2556,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -2581,7 +2582,7 @@
         <v>62</v>
       </c>
       <c r="P14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2595,10 +2596,10 @@
         <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -2608,7 +2609,7 @@
         <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I15">
         <f>3/F15</f>
@@ -2637,7 +2638,7 @@
         <v>65</v>
       </c>
       <c r="P15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2651,10 +2652,10 @@
         <v>45</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F16">
         <v>23</v>
@@ -2664,7 +2665,7 @@
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I16" s="3">
         <f>12/F16</f>
@@ -2693,7 +2694,7 @@
         <v>68</v>
       </c>
       <c r="P16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2707,10 +2708,10 @@
         <v>69</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F17">
         <v>23</v>
@@ -2720,7 +2721,7 @@
         <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I17" s="3">
         <f>11/F17</f>
@@ -2749,7 +2750,7 @@
         <v>72</v>
       </c>
       <c r="P17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2763,10 +2764,10 @@
         <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F18">
         <v>33</v>
@@ -2776,7 +2777,7 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I18" s="3">
         <f>15/F18</f>
@@ -2805,7 +2806,7 @@
         <v>75</v>
       </c>
       <c r="P18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2819,10 +2820,10 @@
         <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2832,7 +2833,7 @@
         <v>23</v>
       </c>
       <c r="H19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2859,7 +2860,7 @@
         <v>77</v>
       </c>
       <c r="P19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2873,10 +2874,10 @@
         <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F20">
         <v>36</v>
@@ -2886,7 +2887,7 @@
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I20" s="3">
         <f>18/F20</f>
@@ -2915,7 +2916,7 @@
         <v>80</v>
       </c>
       <c r="P20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2932,7 +2933,7 @@
         <v>83</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2966,7 +2967,7 @@
         <v>85</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2997,7 +2998,7 @@
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F23">
         <v>9</v>
@@ -3007,7 +3008,7 @@
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I23" s="3">
         <f>9/G23</f>
@@ -3036,7 +3037,7 @@
         <v>89</v>
       </c>
       <c r="P23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -3053,7 +3054,7 @@
         <v>92</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -3087,7 +3088,7 @@
         <v>96</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -3121,7 +3122,7 @@
         <v>100</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -3155,7 +3156,7 @@
         <v>102</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -3186,10 +3187,10 @@
         <v>105</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F28">
         <v>14</v>
@@ -3199,7 +3200,7 @@
         <v>13</v>
       </c>
       <c r="H28" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I28" s="3">
         <f>5/F28</f>
@@ -3228,7 +3229,7 @@
         <v>108</v>
       </c>
       <c r="P28" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -3242,10 +3243,10 @@
         <v>109</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F29">
         <v>25</v>
@@ -3255,7 +3256,7 @@
         <v>18</v>
       </c>
       <c r="H29" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I29" s="3">
         <f>11/F29</f>
@@ -3295,10 +3296,10 @@
         <v>114</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -3308,7 +3309,7 @@
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I30" s="3">
         <f>3/F30</f>
@@ -3337,7 +3338,7 @@
         <v>117</v>
       </c>
       <c r="P30" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -3354,7 +3355,7 @@
         <v>120</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3388,7 +3389,7 @@
         <v>123</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -3422,7 +3423,7 @@
         <v>125</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -3456,7 +3457,7 @@
         <v>129</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -3490,7 +3491,7 @@
         <v>133</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -3521,7 +3522,7 @@
         <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F36">
         <v>15</v>
@@ -3541,10 +3542,10 @@
         <v>139</v>
       </c>
       <c r="P36" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="Q36" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -3558,10 +3559,10 @@
         <v>136</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -3571,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -3598,7 +3599,7 @@
         <v>141</v>
       </c>
       <c r="P37" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3615,7 +3616,7 @@
         <v>142</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -3646,7 +3647,7 @@
         <v>144</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F39">
         <v>5</v>
@@ -3656,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I39" s="3">
         <f>5/F39</f>
@@ -3685,7 +3686,7 @@
         <v>147</v>
       </c>
       <c r="P39" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -3699,10 +3700,10 @@
         <v>45</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -3712,7 +3713,7 @@
         <v>15</v>
       </c>
       <c r="H40" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I40" s="3">
         <f>1/F40</f>
@@ -3741,7 +3742,7 @@
         <v>150</v>
       </c>
       <c r="P40" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3755,7 +3756,7 @@
         <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -3765,7 +3766,7 @@
         <v>2</v>
       </c>
       <c r="H41" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I41" s="3">
         <f>2/F41</f>
@@ -3794,7 +3795,7 @@
         <v>153</v>
       </c>
       <c r="P41" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -3808,10 +3809,10 @@
         <v>154</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F42">
         <v>7</v>
@@ -3821,7 +3822,7 @@
         <v>8</v>
       </c>
       <c r="H42" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I42" s="3">
         <f>7/F42</f>
@@ -3850,7 +3851,7 @@
         <v>157</v>
       </c>
       <c r="P42" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3864,7 +3865,7 @@
         <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F43">
         <v>14</v>
@@ -3874,7 +3875,7 @@
         <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I43" s="3">
         <f>14/F43</f>
@@ -3914,10 +3915,10 @@
         <v>161</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F44">
         <v>16</v>
@@ -3927,7 +3928,7 @@
         <v>19</v>
       </c>
       <c r="H44" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I44" s="3">
         <f>16/F44</f>
@@ -3956,7 +3957,7 @@
         <v>164</v>
       </c>
       <c r="P44" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3970,7 +3971,7 @@
         <v>136</v>
       </c>
       <c r="D45" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F45">
         <v>10</v>
@@ -3980,7 +3981,7 @@
         <v>10</v>
       </c>
       <c r="H45" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I45" s="3">
         <f>10/F45</f>
@@ -4009,7 +4010,7 @@
         <v>167</v>
       </c>
       <c r="P45" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -4023,10 +4024,10 @@
         <v>144</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -4036,7 +4037,7 @@
         <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I46" s="3">
         <f>0/F46</f>
@@ -4064,7 +4065,7 @@
         <v>170</v>
       </c>
       <c r="P46" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -4078,7 +4079,7 @@
         <v>144</v>
       </c>
       <c r="D47" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F47">
         <v>3</v>
@@ -4088,7 +4089,7 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I47" s="3">
         <f>3/F47</f>
@@ -4117,7 +4118,7 @@
         <v>173</v>
       </c>
       <c r="P47" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -4131,7 +4132,7 @@
         <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F48">
         <v>11</v>
@@ -4141,7 +4142,7 @@
         <v>11</v>
       </c>
       <c r="H48" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I48" s="3">
         <f>11/F48</f>
@@ -4170,7 +4171,7 @@
         <v>176</v>
       </c>
       <c r="P48" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -4184,7 +4185,7 @@
         <v>177</v>
       </c>
       <c r="D49" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -4194,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I49" s="3">
         <f>1/1</f>
@@ -4223,7 +4224,7 @@
         <v>180</v>
       </c>
       <c r="P49" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -4237,10 +4238,10 @@
         <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -4260,10 +4261,10 @@
         <v>182</v>
       </c>
       <c r="P50" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Q50" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -4277,7 +4278,7 @@
         <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F51">
         <v>5</v>
@@ -4287,7 +4288,7 @@
         <v>5</v>
       </c>
       <c r="H51" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I51" s="9">
         <v>1</v>
@@ -4314,7 +4315,7 @@
         <v>186</v>
       </c>
       <c r="P51" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -4331,7 +4332,7 @@
         <v>188</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -4365,7 +4366,7 @@
         <v>191</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -4398,6 +4399,9 @@
       <c r="D54" t="s">
         <v>195</v>
       </c>
+      <c r="E54" s="7" t="s">
+        <v>370</v>
+      </c>
       <c r="F54">
         <v>0</v>
       </c>
@@ -4429,6 +4433,9 @@
       <c r="D55" t="s">
         <v>199</v>
       </c>
+      <c r="E55" s="7" t="s">
+        <v>370</v>
+      </c>
       <c r="F55">
         <v>0</v>
       </c>
@@ -4458,10 +4465,10 @@
         <v>202</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F56">
         <v>23</v>
@@ -4471,7 +4478,7 @@
         <v>10</v>
       </c>
       <c r="H56" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I56" s="3">
         <f>3/F56</f>
@@ -4500,7 +4507,7 @@
         <v>205</v>
       </c>
       <c r="P56" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -4514,10 +4521,10 @@
         <v>207</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F57">
         <v>38</v>
@@ -4527,7 +4534,7 @@
         <v>34</v>
       </c>
       <c r="H57" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I57" s="3">
         <f>14/F57</f>
@@ -4556,7 +4563,7 @@
         <v>210</v>
       </c>
       <c r="P57" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -4601,10 +4608,10 @@
         <v>212</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -4614,7 +4621,7 @@
         <v>11</v>
       </c>
       <c r="H59" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I59" s="3">
         <v>0</v>
@@ -4641,7 +4648,7 @@
         <v>215</v>
       </c>
       <c r="P59" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -4655,10 +4662,10 @@
         <v>216</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -4668,7 +4675,7 @@
         <v>15</v>
       </c>
       <c r="H60" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I60" s="3">
         <v>0</v>
@@ -4706,7 +4713,7 @@
         <v>220</v>
       </c>
       <c r="D61" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F61">
         <v>2</v>
@@ -4716,7 +4723,7 @@
         <v>3</v>
       </c>
       <c r="H61" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -4752,10 +4759,10 @@
         <v>224</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -4765,7 +4772,7 @@
         <v>4</v>
       </c>
       <c r="H62" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I62" s="3">
         <v>1</v>
@@ -4798,6 +4805,8 @@
     <hyperlink ref="P2" r:id="rId1" xr:uid="{F97D47B1-5FE4-4745-B981-EBF222D57988}"/>
     <hyperlink ref="P3" r:id="rId2" location="JD_9-1B-1" xr:uid="{D2ECCDDA-1188-D042-B250-42F92DFB3DAF}"/>
     <hyperlink ref="P5" r:id="rId3" location="JD_5-1-4" xr:uid="{6E7910B8-EFBE-3445-BB73-8B5906C34C8F}"/>
+    <hyperlink ref="P7" r:id="rId4" location="JD_10-4-1" xr:uid="{54A8B604-2B63-5E4B-85DF-A83E9E1B0DA6}"/>
+    <hyperlink ref="P13" r:id="rId5" xr:uid="{A24D906F-6DBE-BE43-8387-9BC67C5496E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4808,7 +4817,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F62"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6624,7 +6633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ECE6A1-2687-7F4E-B796-2CBAFFF78F4A}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>

</xml_diff>